<commit_message>
CRUD for Task Type List is done
</commit_message>
<xml_diff>
--- a/Documents/WBS/J2EE_30068_AkashChakraborty_WBS.xlsx
+++ b/Documents/WBS/J2EE_30068_AkashChakraborty_WBS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9215"/>
+    <workbookView windowWidth="11520" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -115,7 +115,7 @@
     <t>3.1.2 Analyze all available API endpoints</t>
   </si>
   <si>
-    <t>3.1.3 Find required enpoints for features</t>
+    <t>3.1.3 Find required endpoints for features</t>
   </si>
   <si>
     <t>3.2 Designed Based on API</t>
@@ -267,11 +267,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="m/d/yyyy;@"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -298,18 +298,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -328,23 +321,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -352,15 +329,31 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -397,16 +390,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -421,7 +421,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -436,7 +436,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -463,187 +463,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -756,21 +756,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -791,6 +776,17 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -821,11 +817,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -844,27 +853,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -874,130 +874,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1016,7 +1016,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1028,7 +1028,7 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1043,7 +1043,7 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1064,7 +1064,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1445,8 +1445,8 @@
   <sheetPr/>
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>

</xml_diff>